<commit_message>
Update Dekhi Bangladesh Bug Report.xlsx
</commit_message>
<xml_diff>
--- a/Dekhi Bangladesh Bug Report.xlsx
+++ b/Dekhi Bangladesh Bug Report.xlsx
@@ -1030,12 +1030,13 @@
     </r>
   </si>
   <si>
+    <t>Screenshot: comment functionality under post does not work</t>
+  </si>
+  <si>
     <t>1. Enter the site url.
-2. Go to a post &amp; scroll down to the comment section
-2. Try to post a comment.</t>
-  </si>
-  <si>
-    <t>Screenshot: comment functionality under post does not work</t>
+2. Go to a post or go to the url: https://db.bpwork.xyz/pages/lalbagh.html
+3.  Scroll down to the comment section.
+4. Try to post a comment.</t>
   </si>
 </sst>
 </file>
@@ -1691,8 +1692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="H108" sqref="H108"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="H109" sqref="H109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2987,7 +2988,7 @@
       </c>
       <c r="F108" s="2"/>
       <c r="H108" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I108" s="2"/>
     </row>
@@ -3015,7 +3016,7 @@
       </c>
       <c r="F110" s="2"/>
       <c r="H110" s="5" t="s">
-        <v>36</v>
+        <v>123</v>
       </c>
       <c r="I110" s="2"/>
     </row>
@@ -3042,8 +3043,8 @@
         <v>121</v>
       </c>
       <c r="F112" s="2"/>
-      <c r="H112" s="8" t="s">
-        <v>138</v>
+      <c r="H112" s="7" t="s">
+        <v>137</v>
       </c>
       <c r="I112" s="2"/>
     </row>
@@ -4059,10 +4060,10 @@
     <hyperlink ref="H100" r:id="rId23"/>
     <hyperlink ref="B112" r:id="rId24"/>
     <hyperlink ref="E112" r:id="rId25"/>
-    <hyperlink ref="H112" r:id="rId26" display="Screenshot: button problem in post page sidebar"/>
+    <hyperlink ref="H112" r:id="rId26"/>
     <hyperlink ref="H88" r:id="rId27" display="Screenshot: button problem in post page sidebar"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait" r:id="rId28"/>
+  <pageSetup orientation="landscape" r:id="rId28"/>
 </worksheet>
 </file>
</xml_diff>